<commit_message>
Fixed image crop and added Kai.
</commit_message>
<xml_diff>
--- a/src/data/current_data/bios_currentdata.xlsx
+++ b/src/data/current_data/bios_currentdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicalin/dsp_vs_code/dspuci-website-gatsby/src/data/current_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE479410-9A21-BD4C-977F-CFB24AB17A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C938D738-FA22-5F46-B9EE-67114BAF4D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="740" windowWidth="26160" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="585">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1754,6 +1754,27 @@
   </si>
   <si>
     <t>Undergraduate Student Assistant @ Merage</t>
+  </si>
+  <si>
+    <t>Kai</t>
+  </si>
+  <si>
+    <t>Bussey</t>
+  </si>
+  <si>
+    <t>kai_bussey</t>
+  </si>
+  <si>
+    <t>Palo Alto, CA</t>
+  </si>
+  <si>
+    <t>Finance, Private Equity, Banking</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kai-bussey-a92008233/</t>
+  </si>
+  <si>
+    <t>kaibussey@ucidsp.com</t>
   </si>
 </sst>
 </file>
@@ -2190,13 +2211,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10:P11"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2501,13 +2522,13 @@
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="11" t="s">
-        <v>520</v>
+        <v>578</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>521</v>
+        <v>579</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>522</v>
+        <v>580</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>478</v>
@@ -2516,709 +2537,707 @@
         <v>479</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>330</v>
+        <v>581</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>523</v>
+        <v>582</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N8" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>526</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P8" s="16" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
+    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
         <v>44404.857638888891</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="B9" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>235</v>
+        <v>85</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>227</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>236</v>
+        <v>23</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>507</v>
+        <v>30</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>508</v>
+        <v>289</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>509</v>
+        <v>86</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>233</v>
+        <v>26</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>510</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>207</v>
+        <v>235</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>208</v>
+        <v>236</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>321</v>
+        <v>507</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>322</v>
+        <v>508</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="M10" t="s">
+        <v>509</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>323</v>
+        <v>510</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>166</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>208</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>487</v>
+        <v>118</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>298</v>
+        <v>209</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>488</v>
+        <v>321</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>489</v>
+        <v>322</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>16</v>
+        <v>210</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>168</v>
+        <v>212</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>169</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>166</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>24</v>
+        <v>487</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>40</v>
+        <v>298</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>180</v>
+        <v>488</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>181</v>
+        <v>297</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>183</v>
+        <v>16</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>438</v>
+        <v>177</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>439</v>
+        <v>178</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>440</v>
+        <v>179</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>329</v>
+        <v>166</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="L14" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="N14" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O14" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P14" s="11" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
+    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
         <v>44404.652777777781</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="N15" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="O15" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="15">
+    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="15">
         <v>44397.381944444445</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N16" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="O16" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="2" t="s">
+    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="B17" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N17" t="s">
         <v>260</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O17" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>568</v>
+        <v>198</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>569</v>
+        <v>199</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>570</v>
+        <v>200</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>478</v>
+        <v>166</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>571</v>
+        <v>201</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>572</v>
+        <v>303</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>576</v>
+        <v>385</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>577</v>
+        <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>21</v>
+        <v>202</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N18" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="O18" s="8" t="s">
-        <v>574</v>
+      <c r="N18" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.15">
-      <c r="A19" s="15">
-        <v>44397.802083333336</v>
-      </c>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>109</v>
+        <v>568</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>569</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>110</v>
+        <v>570</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>45</v>
+        <v>478</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>32</v>
+        <v>571</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>292</v>
+      <c r="I19" s="13" t="s">
+        <v>572</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>308</v>
+        <v>576</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>309</v>
+        <v>577</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>310</v>
+        <v>21</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N19" t="s">
-        <v>111</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>112</v>
+        <v>20</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>574</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="15">
+        <v>44397.802083333336</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>137</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="11" t="s">
+        <v>292</v>
+      </c>
       <c r="J20" s="2" t="s">
-        <v>499</v>
+        <v>308</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>21</v>
+        <v>309</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>140</v>
+        <v>39</v>
+      </c>
+      <c r="N20" t="s">
+        <v>111</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>382</v>
+        <v>136</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>383</v>
+        <v>137</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>384</v>
+        <v>138</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>329</v>
+        <v>116</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>385</v>
+        <v>499</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>386</v>
+        <v>21</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>389</v>
+        <v>16</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>511</v>
+        <v>382</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>122</v>
+        <v>383</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>512</v>
+        <v>384</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>478</v>
+        <v>329</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>14</v>
@@ -3229,223 +3248,225 @@
       <c r="H22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>513</v>
+        <v>385</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>21</v>
+        <v>386</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>515</v>
+        <v>33</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>387</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>516</v>
+        <v>388</v>
       </c>
       <c r="P22" s="16" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>121</v>
+        <v>511</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>122</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>123</v>
+        <v>512</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>116</v>
+        <v>478</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>287</v>
+        <v>40</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>468</v>
-      </c>
-      <c r="L23" s="10" t="s">
-        <v>500</v>
+        <v>513</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N23" t="s">
-        <v>149</v>
+      <c r="N23" s="4" t="s">
+        <v>515</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>516</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>268</v>
+        <v>121</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>269</v>
+        <v>122</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E24" t="s">
-        <v>227</v>
+        <v>123</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>271</v>
+        <v>124</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="J24" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>529</v>
+        <v>467</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>500</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>273</v>
+        <v>35</v>
+      </c>
+      <c r="N24" t="s">
+        <v>149</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>272</v>
+        <v>125</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>530</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B25" s="2" t="s">
-        <v>501</v>
+        <v>268</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>502</v>
+        <v>269</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>478</v>
+        <v>270</v>
+      </c>
+      <c r="E25" t="s">
+        <v>227</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>361</v>
+        <v>271</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>107</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>46</v>
+        <v>528</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>21</v>
+        <v>473</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>472</v>
+        <v>529</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>506</v>
+        <v>273</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>505</v>
+        <v>272</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>504</v>
+        <v>530</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="B27" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="K26" s="16" t="s">
-        <v>474</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>418</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N26" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="O26" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.15">
-      <c r="B27" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>329</v>
@@ -3454,1525 +3475,1571 @@
         <v>27</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="16" t="s">
-        <v>471</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="M27" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>355</v>
+        <v>419</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="P27" s="16" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>420</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
-        <v>237</v>
+        <v>352</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>114</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>431</v>
+        <v>353</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>329</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="16" t="s">
-        <v>433</v>
-      </c>
-      <c r="K28" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>436</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>437</v>
+        <v>472</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>356</v>
       </c>
       <c r="P28" s="16" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>114</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>407</v>
+        <v>431</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>329</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>408</v>
+        <v>14</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>277</v>
+        <v>433</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N29" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>412</v>
+        <v>26</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>437</v>
       </c>
       <c r="P29" s="16" t="s">
-        <v>413</v>
+        <v>435</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>113</v>
+        <v>406</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>114</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>115</v>
+        <v>407</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>116</v>
+        <v>329</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>117</v>
+        <v>15</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>118</v>
       </c>
       <c r="I30" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="P30" s="16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="O30" s="5" t="s">
+      <c r="O31" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="P31" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="I31" t="s">
-        <v>195</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N31" t="s">
-        <v>196</v>
-      </c>
-      <c r="O31" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
-        <v>390</v>
+        <v>190</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>128</v>
+        <v>191</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>391</v>
+        <v>192</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>329</v>
+        <v>166</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>393</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>222</v>
+        <v>193</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I32" t="s">
+        <v>195</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>537</v>
+        <v>21</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>285</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="N32" t="s">
-        <v>395</v>
+        <v>196</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>396</v>
+        <v>197</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>543</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
-        <v>127</v>
+        <v>390</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>129</v>
+        <v>391</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>116</v>
+        <v>329</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>300</v>
+        <v>392</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>301</v>
+        <v>394</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>537</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="N33" t="s">
-        <v>148</v>
+        <v>395</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>131</v>
+        <v>396</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>221</v>
+        <v>543</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
-        <v>372</v>
+        <v>127</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>373</v>
+        <v>128</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>374</v>
+        <v>129</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>329</v>
+        <v>116</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16" t="s">
-        <v>376</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>380</v>
-      </c>
-      <c r="M34" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="M34" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N34" t="s">
-        <v>378</v>
+        <v>148</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="P34" s="16" t="s">
-        <v>381</v>
+        <v>131</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
-        <v>553</v>
+        <v>372</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>554</v>
+        <v>373</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>555</v>
+        <v>374</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>478</v>
+        <v>329</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>361</v>
+        <v>117</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>106</v>
+        <v>375</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="16" t="s">
-        <v>556</v>
+        <v>376</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>21</v>
+        <v>377</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>472</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>559</v>
+        <v>380</v>
+      </c>
+      <c r="M35" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N35" t="s">
+        <v>378</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>558</v>
+        <v>379</v>
       </c>
       <c r="P35" s="16" t="s">
-        <v>557</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="2" t="s">
-        <v>343</v>
+        <v>553</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>344</v>
+        <v>554</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>345</v>
+        <v>555</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>329</v>
+        <v>478</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>348</v>
+        <v>361</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>472</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" t="s">
-        <v>349</v>
+        <v>22</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>559</v>
       </c>
       <c r="O36" s="7" t="s">
-        <v>350</v>
+        <v>558</v>
       </c>
       <c r="P36" s="16" t="s">
-        <v>351</v>
+        <v>557</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="2" t="s">
-        <v>245</v>
+        <v>343</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>246</v>
+        <v>344</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>248</v>
+        <v>345</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>227</v>
+        <v>329</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>405</v>
+        <v>36</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>316</v>
+        <v>107</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>318</v>
+        <v>347</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>319</v>
+        <v>348</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="N37" t="s">
-        <v>249</v>
+        <v>349</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>251</v>
+        <v>350</v>
+      </c>
+      <c r="P37" s="16" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>132</v>
+        <v>245</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>133</v>
+        <v>246</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>55</v>
+        <v>255</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38" s="2"/>
+        <v>405</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>316</v>
+      </c>
       <c r="J38" s="2" t="s">
-        <v>46</v>
+        <v>317</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>21</v>
+        <v>319</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="O38" s="5" t="s">
-        <v>135</v>
+        <v>31</v>
+      </c>
+      <c r="N38" t="s">
+        <v>249</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>274</v>
+        <v>132</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>278</v>
+        <v>133</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>279</v>
+        <v>134</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>280</v>
+        <v>55</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>281</v>
+        <v>46</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>453</v>
+        <v>320</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>277</v>
+        <v>21</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N39" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>275</v>
+      <c r="N39" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
-        <v>422</v>
+        <v>274</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>423</v>
+        <v>278</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>424</v>
+        <v>279</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>329</v>
+        <v>227</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>425</v>
+        <v>280</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="2"/>
+      <c r="I40" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="J40" s="2" t="s">
-        <v>426</v>
+        <v>281</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="L40" s="16" t="s">
-        <v>427</v>
+        <v>453</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="O40" s="12" t="s">
-        <v>429</v>
+        <v>315</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>430</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>531</v>
+        <v>422</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>532</v>
+        <v>423</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>533</v>
+        <v>424</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>478</v>
+        <v>329</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>479</v>
+        <v>14</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>534</v>
+        <v>425</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>535</v>
+        <v>426</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>21</v>
+        <v>463</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>538</v>
+        <v>428</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>539</v>
+        <v>429</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>536</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>531</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>226</v>
+        <v>533</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>227</v>
+        <v>478</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>14</v>
+        <v>479</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>517</v>
+        <v>534</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
-        <v>426</v>
+        <v>535</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>519</v>
+        <v>21</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>418</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N42" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>230</v>
+      <c r="N42" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>539</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>231</v>
+        <v>536</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3">
-        <v>44396.994444444441</v>
-      </c>
+      <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>48</v>
+        <v>540</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>49</v>
+        <v>226</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>45</v>
+        <v>227</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>34</v>
+        <v>517</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>225</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
-        <v>159</v>
+        <v>426</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>469</v>
+        <v>518</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>50</v>
+        <v>519</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N43" s="6" t="s">
+      <c r="N43" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>44396.994444444441</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N44" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="O43" s="5" t="s">
+      <c r="O44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P43" s="2" t="s">
+      <c r="P44" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3"/>
-      <c r="B44" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>565</v>
-      </c>
-      <c r="O44" s="12" t="s">
-        <v>566</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="2" t="s">
-        <v>142</v>
+        <v>560</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>143</v>
+        <v>561</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>144</v>
+        <v>562</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>116</v>
+        <v>478</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>18</v>
+        <v>479</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>145</v>
+        <v>330</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>19</v>
+        <v>563</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2" t="s">
-        <v>426</v>
+        <v>564</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>455</v>
+        <v>21</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>311</v>
+        <v>21</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N45" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>146</v>
+        <v>26</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="O45" s="12" t="s">
+        <v>566</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>456</v>
+        <v>567</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="2" t="s">
-        <v>364</v>
+        <v>142</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>365</v>
+        <v>143</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>366</v>
+        <v>144</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>329</v>
+        <v>116</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>367</v>
+        <v>145</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="K46" s="16" t="s">
-        <v>369</v>
+        <v>426</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>455</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>541</v>
+        <v>311</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="O46" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="P46" s="16" t="s">
-        <v>542</v>
+        <v>152</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="2" t="s">
-        <v>490</v>
+        <v>364</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>491</v>
+        <v>365</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>492</v>
+        <v>366</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>478</v>
+        <v>329</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>479</v>
+        <v>14</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>493</v>
+        <v>367</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2" t="s">
-        <v>108</v>
+        <v>368</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>21</v>
+        <v>369</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>21</v>
+        <v>541</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>495</v>
+        <v>371</v>
       </c>
       <c r="O47" s="12" t="s">
-        <v>496</v>
+        <v>370</v>
       </c>
       <c r="P47" s="16" t="s">
-        <v>494</v>
+        <v>542</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
-        <v>544</v>
+        <v>490</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>545</v>
+        <v>491</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>546</v>
+        <v>492</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>478</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>14</v>
+        <v>479</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>34</v>
+        <v>493</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2" t="s">
-        <v>547</v>
+        <v>108</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>552</v>
+        <v>21</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>548</v>
+        <v>21</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N48" s="12" t="s">
-        <v>549</v>
+        <v>22</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>495</v>
       </c>
       <c r="O48" s="12" t="s">
-        <v>550</v>
+        <v>496</v>
       </c>
       <c r="P48" s="16" t="s">
-        <v>551</v>
+        <v>494</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
       <c r="B49" s="2" t="s">
-        <v>333</v>
+        <v>544</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>334</v>
+        <v>545</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>335</v>
+        <v>546</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>329</v>
+        <v>478</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>336</v>
+        <v>34</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2" t="s">
-        <v>337</v>
+        <v>547</v>
       </c>
       <c r="K49" s="16" t="s">
-        <v>338</v>
+        <v>552</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>339</v>
+        <v>548</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N49" s="4" t="s">
-        <v>342</v>
+        <v>20</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>549</v>
       </c>
       <c r="O49" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="3">
-        <v>44409.992361111108</v>
-      </c>
+        <v>550</v>
+      </c>
+      <c r="P49" s="16" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="3"/>
       <c r="B50" s="2" t="s">
-        <v>71</v>
+        <v>333</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>72</v>
+        <v>334</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>73</v>
+        <v>335</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>54</v>
+        <v>329</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>42</v>
+        <v>336</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>291</v>
+        <v>337</v>
+      </c>
+      <c r="K50" s="16" t="s">
+        <v>338</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>21</v>
+        <v>339</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>75</v>
+        <v>342</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>341</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>160</v>
+        <v>340</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="3"/>
+      <c r="A51" s="3">
+        <v>44409.992361111108</v>
+      </c>
       <c r="B51" s="2" t="s">
-        <v>261</v>
+        <v>71</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>262</v>
+        <v>72</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>263</v>
+        <v>73</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>227</v>
+        <v>54</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>264</v>
+        <v>42</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
-        <v>465</v>
+        <v>108</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>265</v>
+        <v>21</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>267</v>
+        <v>74</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>266</v>
+        <v>75</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="3"/>
       <c r="B52" s="2" t="s">
-        <v>170</v>
+        <v>261</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>104</v>
+        <v>262</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>171</v>
+        <v>263</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H52" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I52" t="s">
-        <v>172</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>173</v>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2" t="s">
+        <v>465</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="L52" s="11" t="s">
-        <v>294</v>
+        <v>304</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N52" t="s">
-        <v>175</v>
-      </c>
-      <c r="O52" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="P52" s="13" t="s">
-        <v>174</v>
+        <v>41</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>238</v>
+      <c r="B53" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>239</v>
+        <v>171</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I53" s="11"/>
+      <c r="G53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I53" t="s">
+        <v>172</v>
+      </c>
       <c r="J53" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="K53" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="L53" s="13" t="s">
-        <v>241</v>
+        <v>173</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="L53" s="11" t="s">
+        <v>294</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N53" t="s">
-        <v>242</v>
+        <v>175</v>
       </c>
       <c r="O53" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>244</v>
+        <v>176</v>
+      </c>
+      <c r="P53" s="13" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="15">
-        <v>44397.036111111112</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>58</v>
+      <c r="B54" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>238</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>59</v>
+        <v>239</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>45</v>
+        <v>227</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>29</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="11"/>
       <c r="J54" s="11" t="s">
-        <v>30</v>
+        <v>324</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>464</v>
-      </c>
-      <c r="L54" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M54" s="11" t="s">
-        <v>20</v>
+        <v>462</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="N54" t="s">
-        <v>61</v>
-      </c>
-      <c r="O54" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="P54" s="13" t="s">
-        <v>63</v>
+        <v>242</v>
+      </c>
+      <c r="O54" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15">
-        <v>44411.775694444441</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>77</v>
+        <v>44397.036111111112</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="2"/>
+        <v>29</v>
+      </c>
       <c r="J55" s="11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>450</v>
-      </c>
-      <c r="L55" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="L55" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M55" s="11" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="N55" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="O55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="P55" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="2" t="s">
-        <v>213</v>
+        <v>62</v>
+      </c>
+      <c r="P55" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="15">
+        <v>44411.775694444441</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>166</v>
+        <v>54</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I56" t="s">
-        <v>172</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I56" s="2"/>
       <c r="J56" s="11" t="s">
-        <v>302</v>
+        <v>38</v>
       </c>
       <c r="K56" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="L56" s="11" t="s">
-        <v>216</v>
+        <v>450</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="M56" s="11" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="N56" t="s">
-        <v>217</v>
-      </c>
-      <c r="O56" s="12" t="s">
-        <v>218</v>
+        <v>80</v>
+      </c>
+      <c r="O56" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I57" t="s">
+        <v>172</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="L57" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="M57" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N57" t="s">
+        <v>217</v>
+      </c>
+      <c r="O57" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G58" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="J57" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="K57" s="16" t="s">
-        <v>497</v>
-      </c>
-      <c r="L57" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="M57" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N57" t="s">
-        <v>362</v>
-      </c>
-      <c r="O57" s="12" t="s">
-        <v>363</v>
-      </c>
-      <c r="P57" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="15">
-        <v>44405.647916666669</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="H58" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="J58" s="11" t="s">
+      <c r="J58" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K58" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="L58" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="M58" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" t="s">
+        <v>362</v>
+      </c>
+      <c r="O58" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="15">
+        <v>44405.647916666669</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K58" s="11" t="s">
+      <c r="K59" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="L58" s="13" t="s">
+      <c r="L59" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="M58" s="11" t="s">
+      <c r="M59" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N59" t="s">
         <v>95</v>
       </c>
-      <c r="O58" s="12" t="s">
+      <c r="O59" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="P58" s="2" t="s">
+      <c r="P59" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
+    <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:P51">
-    <sortCondition ref="C4:C51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:P52">
+    <sortCondition ref="C4:C52"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="N39" r:id="rId1" xr:uid="{CBF3488F-0731-4784-B778-22BEDC9A87FD}"/>
+    <hyperlink ref="N40" r:id="rId1" xr:uid="{CBF3488F-0731-4784-B778-22BEDC9A87FD}"/>
     <hyperlink ref="O6" r:id="rId2" xr:uid="{AA553A20-924A-4A7A-B3C1-6D6F29D53AB7}"/>
-    <hyperlink ref="O49" r:id="rId3" xr:uid="{9F78E4A3-9753-40AC-9C13-EFA682AF983E}"/>
-    <hyperlink ref="O36" r:id="rId4" xr:uid="{C0B53B11-AD93-46B5-9A27-594CC3A5271C}"/>
-    <hyperlink ref="N27" r:id="rId5" xr:uid="{19C35423-B41E-431E-A7D2-61DD10A2F89A}"/>
-    <hyperlink ref="O27" r:id="rId6" xr:uid="{FE29F50A-8A83-4CCD-A9E1-9EC92A26530E}"/>
-    <hyperlink ref="O57" r:id="rId7" xr:uid="{365E22B1-13F2-4C32-B64B-BC5B771A124E}"/>
-    <hyperlink ref="O46" r:id="rId8" xr:uid="{EE808F38-5A70-43A7-B847-4DFEFF8C2345}"/>
-    <hyperlink ref="O34" r:id="rId9" xr:uid="{C7957FDB-9E17-4A60-BBEB-6ACA89C74CF0}"/>
-    <hyperlink ref="O21" r:id="rId10" xr:uid="{F34024D8-C79C-4E14-91EB-C1D38E6B185F}"/>
-    <hyperlink ref="O32" r:id="rId11" xr:uid="{A8E15ABD-7D2B-4B1E-90AD-87A935FE52C9}"/>
+    <hyperlink ref="O50" r:id="rId3" xr:uid="{9F78E4A3-9753-40AC-9C13-EFA682AF983E}"/>
+    <hyperlink ref="O37" r:id="rId4" xr:uid="{C0B53B11-AD93-46B5-9A27-594CC3A5271C}"/>
+    <hyperlink ref="N28" r:id="rId5" xr:uid="{19C35423-B41E-431E-A7D2-61DD10A2F89A}"/>
+    <hyperlink ref="O28" r:id="rId6" xr:uid="{FE29F50A-8A83-4CCD-A9E1-9EC92A26530E}"/>
+    <hyperlink ref="O58" r:id="rId7" xr:uid="{365E22B1-13F2-4C32-B64B-BC5B771A124E}"/>
+    <hyperlink ref="O47" r:id="rId8" xr:uid="{EE808F38-5A70-43A7-B847-4DFEFF8C2345}"/>
+    <hyperlink ref="O35" r:id="rId9" xr:uid="{C7957FDB-9E17-4A60-BBEB-6ACA89C74CF0}"/>
+    <hyperlink ref="O22" r:id="rId10" xr:uid="{F34024D8-C79C-4E14-91EB-C1D38E6B185F}"/>
+    <hyperlink ref="O33" r:id="rId11" xr:uid="{A8E15ABD-7D2B-4B1E-90AD-87A935FE52C9}"/>
     <hyperlink ref="O2" r:id="rId12" xr:uid="{9EFE127E-94E1-4D1A-B4FF-56A0D7F365F6}"/>
-    <hyperlink ref="O29" r:id="rId13" xr:uid="{694135F8-96D1-41DA-A6C7-782217CF8081}"/>
-    <hyperlink ref="O26" r:id="rId14" xr:uid="{4AFEC0A6-99D6-4CB4-AA7F-2747B52DE82F}"/>
-    <hyperlink ref="O40" r:id="rId15" xr:uid="{1CF56EA4-06F0-461F-9648-39BB0DCA36A3}"/>
-    <hyperlink ref="N28" r:id="rId16" xr:uid="{59E4A675-78BA-4241-9770-4D060595A68E}"/>
-    <hyperlink ref="O28" r:id="rId17" xr:uid="{3A71C51C-0184-4AC7-AFF4-DD100418FA0C}"/>
-    <hyperlink ref="N13" r:id="rId18" xr:uid="{DFD50037-4AF8-4266-B9E8-32F987D61850}"/>
-    <hyperlink ref="O13" r:id="rId19" xr:uid="{5DDFB26C-A00E-4DCD-860F-446A67100756}"/>
+    <hyperlink ref="O30" r:id="rId13" xr:uid="{694135F8-96D1-41DA-A6C7-782217CF8081}"/>
+    <hyperlink ref="O27" r:id="rId14" xr:uid="{4AFEC0A6-99D6-4CB4-AA7F-2747B52DE82F}"/>
+    <hyperlink ref="O41" r:id="rId15" xr:uid="{1CF56EA4-06F0-461F-9648-39BB0DCA36A3}"/>
+    <hyperlink ref="N29" r:id="rId16" xr:uid="{59E4A675-78BA-4241-9770-4D060595A68E}"/>
+    <hyperlink ref="O29" r:id="rId17" xr:uid="{3A71C51C-0184-4AC7-AFF4-DD100418FA0C}"/>
+    <hyperlink ref="N14" r:id="rId18" xr:uid="{DFD50037-4AF8-4266-B9E8-32F987D61850}"/>
+    <hyperlink ref="O14" r:id="rId19" xr:uid="{5DDFB26C-A00E-4DCD-860F-446A67100756}"/>
     <hyperlink ref="O3" r:id="rId20" xr:uid="{496C672A-A2C0-964F-A09C-3F6E9E54D395}"/>
-    <hyperlink ref="O47" r:id="rId21" xr:uid="{391E2F16-7BE2-BF45-966E-4AA8C82A3A8C}"/>
-    <hyperlink ref="O25" r:id="rId22" xr:uid="{8B4CD950-5E03-BA4C-A31A-6D81180F5668}"/>
-    <hyperlink ref="N25" r:id="rId23" xr:uid="{906C10FB-A487-0F44-B7E6-1ED8FACC4B69}"/>
-    <hyperlink ref="O22" r:id="rId24" xr:uid="{48461CB6-4C2D-4D48-B70F-DE51109A8ABB}"/>
-    <hyperlink ref="N21" r:id="rId25" xr:uid="{3C3E3B29-6A40-184B-8F9A-2CF40AA18114}"/>
-    <hyperlink ref="O7" r:id="rId26" xr:uid="{1C6BEACD-95C4-1B42-8908-9AEE21DD5284}"/>
-    <hyperlink ref="N7" r:id="rId27" xr:uid="{DECFF68F-407D-A64C-AF9F-EA8F0545F147}"/>
-    <hyperlink ref="N41" r:id="rId28" xr:uid="{D26BD10F-086B-144D-9C84-D24073FF3261}"/>
-    <hyperlink ref="O41" r:id="rId29" xr:uid="{4351C873-DDA0-414B-8E8F-F9278C8DB149}"/>
-    <hyperlink ref="N48" r:id="rId30" xr:uid="{8738F935-185E-D04E-8169-FBD0D688BD90}"/>
-    <hyperlink ref="O48" r:id="rId31" xr:uid="{671530BA-A262-094E-9FB1-37C29825A004}"/>
-    <hyperlink ref="O35" r:id="rId32" xr:uid="{E33637EE-2287-C745-85FF-0F0384FCFB54}"/>
-    <hyperlink ref="N35" r:id="rId33" xr:uid="{80DC692F-9332-C846-BF07-47B1F81F0D36}"/>
-    <hyperlink ref="N44" r:id="rId34" xr:uid="{95F7F419-BA04-6042-A79E-712E39587DB9}"/>
-    <hyperlink ref="O44" r:id="rId35" xr:uid="{45263989-7E51-6246-8402-12558CB9EEC1}"/>
-    <hyperlink ref="N18" r:id="rId36" xr:uid="{6A09C08A-8323-7E4A-B3BC-E58498BDEACF}"/>
-    <hyperlink ref="O18" r:id="rId37" xr:uid="{8355733E-07AE-B240-A471-81E622F1BC51}"/>
+    <hyperlink ref="O48" r:id="rId21" xr:uid="{391E2F16-7BE2-BF45-966E-4AA8C82A3A8C}"/>
+    <hyperlink ref="O26" r:id="rId22" xr:uid="{8B4CD950-5E03-BA4C-A31A-6D81180F5668}"/>
+    <hyperlink ref="N26" r:id="rId23" xr:uid="{906C10FB-A487-0F44-B7E6-1ED8FACC4B69}"/>
+    <hyperlink ref="O23" r:id="rId24" xr:uid="{48461CB6-4C2D-4D48-B70F-DE51109A8ABB}"/>
+    <hyperlink ref="N22" r:id="rId25" xr:uid="{3C3E3B29-6A40-184B-8F9A-2CF40AA18114}"/>
+    <hyperlink ref="O8" r:id="rId26" xr:uid="{1C6BEACD-95C4-1B42-8908-9AEE21DD5284}"/>
+    <hyperlink ref="N8" r:id="rId27" xr:uid="{DECFF68F-407D-A64C-AF9F-EA8F0545F147}"/>
+    <hyperlink ref="N42" r:id="rId28" xr:uid="{D26BD10F-086B-144D-9C84-D24073FF3261}"/>
+    <hyperlink ref="O42" r:id="rId29" xr:uid="{4351C873-DDA0-414B-8E8F-F9278C8DB149}"/>
+    <hyperlink ref="N49" r:id="rId30" xr:uid="{8738F935-185E-D04E-8169-FBD0D688BD90}"/>
+    <hyperlink ref="O49" r:id="rId31" xr:uid="{671530BA-A262-094E-9FB1-37C29825A004}"/>
+    <hyperlink ref="O36" r:id="rId32" xr:uid="{E33637EE-2287-C745-85FF-0F0384FCFB54}"/>
+    <hyperlink ref="N36" r:id="rId33" xr:uid="{80DC692F-9332-C846-BF07-47B1F81F0D36}"/>
+    <hyperlink ref="N45" r:id="rId34" xr:uid="{95F7F419-BA04-6042-A79E-712E39587DB9}"/>
+    <hyperlink ref="O45" r:id="rId35" xr:uid="{45263989-7E51-6246-8402-12558CB9EEC1}"/>
+    <hyperlink ref="N19" r:id="rId36" xr:uid="{6A09C08A-8323-7E4A-B3BC-E58498BDEACF}"/>
+    <hyperlink ref="O19" r:id="rId37" xr:uid="{8355733E-07AE-B240-A471-81E622F1BC51}"/>
+    <hyperlink ref="N7" r:id="rId38" xr:uid="{DC07D7C8-1C0A-6E44-AAC8-71BB7F8FC6E2}"/>
+    <hyperlink ref="O7" r:id="rId39" xr:uid="{1BC9CAA2-DBB4-4E4C-A1BB-880A94C27EC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId38"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed forest and julie
</commit_message>
<xml_diff>
--- a/src/data/current_data/bios_currentdata.xlsx
+++ b/src/data/current_data/bios_currentdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicalin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicalin/dsp_vs_code/dspuci-website-gatsby/src/data/current_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5361FEB-A47D-4E42-8638-01C9B17B70D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CECA18-6433-E047-AFBE-C4519F546FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="740" windowWidth="26160" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>foresthuang@ucidsp.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi! I’m Forest Huang and I initiated fall of my freshman year as part of the Alpha Mu class. My favorite pastimes include hanging out with friends, trying new foods/restaurants, and playing/watching Esports. A fun fact about me is that I’ve been to two three Michelin starred restaurants (technically 3 if you count takeout). Ask me about video games, stocks, or anything else during recruitment! </t>
-  </si>
-  <si>
     <t>Julia</t>
   </si>
   <si>
@@ -787,9 +784,6 @@
     <t>juliana_lee</t>
   </si>
   <si>
-    <t>Psychology</t>
-  </si>
-  <si>
     <t>Marketing, UI/UX Design</t>
   </si>
   <si>
@@ -1280,6 +1274,12 @@
   </si>
   <si>
     <t>Software Engineering, Quant</t>
+  </si>
+  <si>
+    <t>Psychology, Digital Arts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi! I’m Forest Huang and I initiated fall of my freshman year as part of the Alpha Mu class. My favorite pastimes include hanging out with friends, trying new foods/restaurants, and playing/watching Esports. A fun fact about me is that I’ve been to two Michelin starred restaurants (technically 3 if you count takeout). Ask me about video games, stocks, or anything else during recruitment! </t>
   </si>
 </sst>
 </file>
@@ -1718,10 +1718,10 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
+      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1794,113 +1794,113 @@
     <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>317</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>59</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>318</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>320</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>26</v>
@@ -1909,172 +1909,172 @@
         <v>27</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N4" t="s">
+        <v>177</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>179</v>
-      </c>
       <c r="P4" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>409</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>411</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="O5" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="P5" s="15" t="s">
         <v>412</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>352</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>59</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="M7" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="O7" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="P7" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>25</v>
@@ -2089,86 +2089,86 @@
         <v>35</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="L9" s="11" t="s">
         <v>290</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>292</v>
       </c>
       <c r="M9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="N9" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="P9" s="11" t="s">
         <v>293</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>14</v>
@@ -2181,58 +2181,58 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="L10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>20</v>
@@ -2241,25 +2241,25 @@
         <v>19</v>
       </c>
       <c r="N11" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>57</v>
@@ -2268,14 +2268,14 @@
         <v>25</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>20</v>
@@ -2287,28 +2287,28 @@
         <v>16</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>14</v>
@@ -2321,40 +2321,40 @@
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N13" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="P13" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>14</v>
@@ -2369,7 +2369,7 @@
         <v>35</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>20</v>
@@ -2381,13 +2381,13 @@
         <v>31</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="P14" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
@@ -2413,93 +2413,93 @@
         <v>18</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>66</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>67</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>51</v>
@@ -2514,83 +2514,83 @@
         <v>20</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N18" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>59</v>
@@ -2599,83 +2599,83 @@
         <v>35</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M19" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N19" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="O19" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="P19" s="15" t="s">
         <v>203</v>
-      </c>
-      <c r="P19" s="15" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="P20" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>25</v>
@@ -2687,28 +2687,28 @@
         <v>59</v>
       </c>
       <c r="I21" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="K21" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="J21" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>257</v>
-      </c>
       <c r="L21" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="P21" s="15" t="s">
         <v>258</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="P21" s="15" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2738,19 +2738,19 @@
         <v>35</v>
       </c>
       <c r="J22" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>61</v>
@@ -2761,104 +2761,104 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I23" t="s">
         <v>105</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I23" t="s">
-        <v>106</v>
-      </c>
       <c r="J23" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N23" t="s">
+        <v>106</v>
+      </c>
+      <c r="O23" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O23" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="P23" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="J24" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J24" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="L24" s="15" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N24" t="s">
+        <v>241</v>
+      </c>
+      <c r="O24" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="O24" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="P24" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>57</v>
@@ -2867,48 +2867,48 @@
         <v>25</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>25</v>
@@ -2917,94 +2917,94 @@
         <v>58</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="K26" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>224</v>
-      </c>
       <c r="L26" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M26" s="15" t="s">
         <v>28</v>
       </c>
       <c r="N26" t="s">
+        <v>224</v>
+      </c>
+      <c r="O26" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="O26" s="7" t="s">
-        <v>226</v>
-      </c>
       <c r="P26" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>384</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H27" s="15" t="s">
         <v>51</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>32</v>
@@ -3013,84 +3013,84 @@
         <v>52</v>
       </c>
       <c r="J28" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N28" t="s">
+        <v>195</v>
+      </c>
+      <c r="O28" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="O28" s="7" t="s">
+      <c r="P28" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="P28" s="15" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N29" t="s">
+        <v>136</v>
+      </c>
+      <c r="O29" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="O29" s="7" t="s">
+      <c r="P29" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>57</v>
@@ -3109,7 +3109,7 @@
         <v>40</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>20</v>
@@ -3118,105 +3118,105 @@
         <v>21</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N31" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="P31" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="O31" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>362</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L32" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3225,44 +3225,44 @@
         <v>49</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>59</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O33" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="O33" s="5" t="s">
+      <c r="P33" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3291,13 +3291,13 @@
         <v>33</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>44</v>
@@ -3318,114 +3318,114 @@
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N35" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="P35" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K36" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="K36" s="15" t="s">
-        <v>216</v>
-      </c>
       <c r="L36" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O36" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P36" s="15" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="E37" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>59</v>
@@ -3444,28 +3444,28 @@
         <v>21</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O37" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="P37" s="15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>375</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>14</v>
@@ -3478,138 +3478,138 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N38" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="P38" s="15" t="s">
         <v>378</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="P38" s="15" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>27</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K39" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="L39" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G40" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40" t="s">
+        <v>92</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L40" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="I40" t="s">
-        <v>93</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="L40" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="M40" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N40" t="s">
+        <v>119</v>
+      </c>
+      <c r="O40" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="O40" s="12" t="s">
+      <c r="P40" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H41" s="11" t="s">
         <v>51</v>
@@ -3618,22 +3618,22 @@
         <v>53</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L41" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="M41" s="11" t="s">
         <v>24</v>
       </c>
       <c r="N41" t="s">
+        <v>208</v>
+      </c>
+      <c r="O41" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="O41" s="12" t="s">
-        <v>210</v>
-      </c>
       <c r="P41" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
updated diana and added 2nd rush app
</commit_message>
<xml_diff>
--- a/src/data/current_data/bios_currentdata.xlsx
+++ b/src/data/current_data/bios_currentdata.xlsx
@@ -562,10 +562,10 @@
     <t>Laguna Hills, CA</t>
   </si>
   <si>
-    <t>Data Analytics, Information Systems, Digital Marketing</t>
-  </si>
-  <si>
-    <t>Data Analytics Intern @ General Atomics Aeronautical Systems, Inc.</t>
+    <t>Data Engineering, Product Management, Marketing</t>
+  </si>
+  <si>
+    <t>Technology Business Office Portfolio Management Intern @ CME Group</t>
   </si>
   <si>
     <t>UCI Women's Club Soccer, Sports Business Association</t>
@@ -1536,15 +1536,15 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000ff"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000ff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1591,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1626,10 +1626,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1637,9 +1637,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1958,22 +1955,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="19" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="17" width="37.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
@@ -2810,7 +2807,7 @@
         <v>199</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="90" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="102" customFormat="1" s="1">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -2860,7 +2857,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="90" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="115.5" customFormat="1" s="1">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>221</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="90" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="88.5" customFormat="1" s="1">
       <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
@@ -2956,7 +2953,7 @@
         <v>231</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="78" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="102" customFormat="1" s="1">
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
@@ -3004,7 +3001,7 @@
         <v>240</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="217.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -3739,7 +3736,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="15" t="s">

</xml_diff>

<commit_message>
fixed how to join revert
</commit_message>
<xml_diff>
--- a/src/data/current_data/bios_currentdata.xlsx
+++ b/src/data/current_data/bios_currentdata.xlsx
@@ -562,10 +562,10 @@
     <t>Laguna Hills, CA</t>
   </si>
   <si>
-    <t>Data Analytics, Information Systems, Digital Marketing</t>
-  </si>
-  <si>
-    <t>Data Analytics Intern @ General Atomics Aeronautical Systems, Inc.</t>
+    <t>Data Engineering, Product Management, Marketing</t>
+  </si>
+  <si>
+    <t>Technology Business Office Portfolio Management Intern @ CME Group</t>
   </si>
   <si>
     <t>UCI Women's Club Soccer, Sports Business Association</t>
@@ -2021,7 +2021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="128.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="127.5" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Updated Website heading into Winter 2025
</commit_message>
<xml_diff>
--- a/src/data/current_data/bios_currentdata.xlsx
+++ b/src/data/current_data/bios_currentdata.xlsx
@@ -339,274 +339,274 @@
     <t>Palo Alto, CA</t>
   </si>
   <si>
-    <t>Economics, Dance</t>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Management, Digital Information Systems</t>
+  </si>
+  <si>
+    <t>Marketing, UI/UX Design, Public Relations</t>
+  </si>
+  <si>
+    <t>Marketing Intern @ Sciframe IO</t>
+  </si>
+  <si>
+    <t>Business Careers in Entertainment Club, Bare Bones Dance Theater</t>
+  </si>
+  <si>
+    <t>Su-Hung-Green</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/siena-dunn/</t>
+  </si>
+  <si>
+    <t>sienadunn@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi! My name is Siena, and I initiated my first year spring with the Alpha Tau class. In my free time, I enjoy dancing, going to concerts, golfing, cooking, and going to the beach. At recruitment, ask me about my favorite shows I’ve binged recently or my favorite matcha spots!</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Guo</t>
+  </si>
+  <si>
+    <t>emily_guo</t>
+  </si>
+  <si>
+    <t>Auckland, New Zealand</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Strategy Intern @ Breez Events and Consulting</t>
+  </si>
+  <si>
+    <t>MAISS, Tennis Club</t>
+  </si>
+  <si>
+    <t>Huang-Merchant</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/emily-guo111/</t>
+  </si>
+  <si>
+    <t>emilyguo@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi! I am Emily and initiated in the spring of my first year. In my free time, I love listening to music, making Pinterest boards and art &amp; fashion. Talk to me about countries I’ve travelled to and my love for The Weeknd and Lana Del Rey!</t>
+  </si>
+  <si>
+    <t>Ayushi</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>ayushi_gupta</t>
+  </si>
+  <si>
+    <t>Alpha Pi</t>
+  </si>
+  <si>
+    <t>Ladera Ranch, CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informatics </t>
+  </si>
+  <si>
+    <t>Finance, Product Management, Data</t>
+  </si>
+  <si>
+    <t>Finance Intern @ Raytheon Technologies</t>
+  </si>
+  <si>
+    <t>UBA</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ayushigupta8/</t>
+  </si>
+  <si>
+    <t>ayushigupta@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hey! My name is Ayushi and I initiated fall quarter of my second year with the Alpha Pi class. I'm a big sports gal and I love to hang out with friends, watch movies, play soccer, get food, and have deep philosophical convos. Feel free to ask me about my favorite foods, tv shows, and goals I have for the rest of the year during recruitment!</t>
+  </si>
+  <si>
+    <t>Coca</t>
+  </si>
+  <si>
+    <t>Ho</t>
+  </si>
+  <si>
+    <t>coca_ho</t>
+  </si>
+  <si>
+    <t>Alpha Omicron</t>
+  </si>
+  <si>
+    <t>Finance, Accounting</t>
+  </si>
+  <si>
+    <t>Consumer Insights Intern @ FOX Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Tennis </t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/coca-ho-a74008269/</t>
+  </si>
+  <si>
+    <t>cocaho@ucidsp.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hey guys! My name is Coca. I am a proud Alpha Omicron and I initiated in the spring of my first year. Some hobbies of mine include tennis, golf, poetry, and oil painting. I love parrots, iced honey lattes, and hot pink! Ask me about why I think listening to music is a waste of time. </t>
+  </si>
+  <si>
+    <t>Ananya</t>
+  </si>
+  <si>
+    <t>Iyengar</t>
+  </si>
+  <si>
+    <t>ananya_iyengar</t>
+  </si>
+  <si>
+    <t>Miami, FL</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Sales, Marketing</t>
+  </si>
+  <si>
+    <t>Client and Product Support Intern @ Origence</t>
+  </si>
+  <si>
+    <t>Indian Subcontinental Club</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ananyaiyengar3/</t>
+  </si>
+  <si>
+    <t>ananyaiyengar@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi! My name is Ananya and I initiated in my sophomore fall with the Alpha Sigma class. In my free time, I love to sing, try new sweet treats, and go to the beach. At recruitment, ask me about my favorite shows to binge-watch and why monkeys are my favorite animals. So excited to meet you all!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shreya </t>
+  </si>
+  <si>
+    <t>Jagannathan</t>
+  </si>
+  <si>
+    <t>shreya_jagannathan</t>
+  </si>
+  <si>
+    <t>San Ramon, CA</t>
+  </si>
+  <si>
+    <t>Business Information Management, Political Science</t>
+  </si>
+  <si>
+    <t>Law, Entrepreneurship, Finance</t>
+  </si>
+  <si>
+    <t>External Relations Assistant @ UCI Libraries</t>
+  </si>
+  <si>
+    <t>ASUCI</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shreyajagan/</t>
+  </si>
+  <si>
+    <t>shreyajagannathan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hey, my name is Shreya! I initiated in the fall quarter of my first year with the Alpha Sigma class. In my free time, I love to read, watch horror movies, and make very specific pinterest boards. Feel free to ask me about places I’ve traveled to and lived in!</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Jukita</t>
+  </si>
+  <si>
+    <t>amelia_jukita</t>
+  </si>
+  <si>
+    <t>Jakarta, Indonesia</t>
+  </si>
+  <si>
+    <t>Product Management</t>
+  </si>
+  <si>
+    <t>Product Management Intern @ Stride</t>
+  </si>
+  <si>
+    <t>180 Degrees Consulting, Product Association, MAISS</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/amelia-jukita/</t>
+  </si>
+  <si>
+    <t>ameliajukita@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hii! My name is Amelia, and I initiated in the fall quarter of my sophomore year with the Alpha Sigma Class. I enjoy thrifting, playing the piano, and exploring new food combinations. Feel free to ask me about my love for harbor seals!</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>Kapadekar</t>
+  </si>
+  <si>
+    <t>riya_kapadekar</t>
+  </si>
+  <si>
+    <t>Informatics</t>
+  </si>
+  <si>
+    <t>Psychology</t>
+  </si>
+  <si>
+    <t>Project Management, Product Management</t>
+  </si>
+  <si>
+    <t>Specialty Masters Program Student Assistant @ Paul Merage School of Business</t>
+  </si>
+  <si>
+    <t>MAISS, Product Association</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/riya-kapadekar/</t>
+  </si>
+  <si>
+    <t>riyakapadekar@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi! My name is Riya and I'm part of the Alpha Sigma class. In my free time, I love going to the beach, making Pinterest boards, and trying new cafes! Ask me about my love for Tru Fru, Lana del Rey, and Grey's Anatomy.</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>james_kent</t>
+  </si>
+  <si>
+    <t>Santa Clarita, CA</t>
   </si>
   <si>
     <t>Management</t>
-  </si>
-  <si>
-    <t>Marketing, UI/UX Design, Public Relations</t>
-  </si>
-  <si>
-    <t>Marketing Intern @ Sciframe IO</t>
-  </si>
-  <si>
-    <t>Business Careers in Entertainment Club, Bare Bones Dance Theater</t>
-  </si>
-  <si>
-    <t>Su-Hung-Green</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/siena-dunn/</t>
-  </si>
-  <si>
-    <t>sienadunn@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hi! My name is Siena, and I initiated my first year spring with the Alpha Tau class. In my free time, I enjoy dancing, going to concerts, golfing, cooking, and going to the beach. At recruitment, ask me about my favorite shows I’ve binged recently or my favorite matcha spots!</t>
-  </si>
-  <si>
-    <t>Emily</t>
-  </si>
-  <si>
-    <t>Guo</t>
-  </si>
-  <si>
-    <t>emily_guo</t>
-  </si>
-  <si>
-    <t>Auckland, New Zealand</t>
-  </si>
-  <si>
-    <t>Consulting</t>
-  </si>
-  <si>
-    <t>Strategy Intern @ Breez Events and Consulting</t>
-  </si>
-  <si>
-    <t>MAISS, Tennis Club</t>
-  </si>
-  <si>
-    <t>Huang-Merchant</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/emily-guo111/</t>
-  </si>
-  <si>
-    <t>emilyguo@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hi! I am Emily and initiated in the spring of my first year. In my free time, I love listening to music, making Pinterest boards and art &amp; fashion. Talk to me about countries I’ve travelled to and my love for The Weeknd and Lana Del Rey!</t>
-  </si>
-  <si>
-    <t>Ayushi</t>
-  </si>
-  <si>
-    <t>Gupta</t>
-  </si>
-  <si>
-    <t>ayushi_gupta</t>
-  </si>
-  <si>
-    <t>Alpha Pi</t>
-  </si>
-  <si>
-    <t>Ladera Ranch, CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informatics </t>
-  </si>
-  <si>
-    <t>Finance, Product Management, Data</t>
-  </si>
-  <si>
-    <t>Finance Intern @ Raytheon Technologies</t>
-  </si>
-  <si>
-    <t>UBA</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ayushigupta8/</t>
-  </si>
-  <si>
-    <t>ayushigupta@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hey! My name is Ayushi and I initiated fall quarter of my second year with the Alpha Pi class. I'm a big sports gal and I love to hang out with friends, watch movies, play soccer, get food, and have deep philosophical convos. Feel free to ask me about my favorite foods, tv shows, and goals I have for the rest of the year during recruitment!</t>
-  </si>
-  <si>
-    <t>Coca</t>
-  </si>
-  <si>
-    <t>Ho</t>
-  </si>
-  <si>
-    <t>coca_ho</t>
-  </si>
-  <si>
-    <t>Alpha Omicron</t>
-  </si>
-  <si>
-    <t>Finance, Accounting</t>
-  </si>
-  <si>
-    <t>Consumer Insights Intern @ FOX Entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Club Tennis </t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/coca-ho-a74008269/</t>
-  </si>
-  <si>
-    <t>cocaho@ucidsp.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hey guys! My name is Coca. I am a proud Alpha Omicron and I initiated in the spring of my first year. Some hobbies of mine include tennis, golf, poetry, and oil painting. I love parrots, iced honey lattes, and hot pink! Ask me about why I think listening to music is a waste of time. </t>
-  </si>
-  <si>
-    <t>Ananya</t>
-  </si>
-  <si>
-    <t>Iyengar</t>
-  </si>
-  <si>
-    <t>ananya_iyengar</t>
-  </si>
-  <si>
-    <t>Miami, FL</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>Sales, Marketing</t>
-  </si>
-  <si>
-    <t>Client and Product Support Intern @ Origence</t>
-  </si>
-  <si>
-    <t>Indian Subcontinental Club</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ananyaiyengar3/</t>
-  </si>
-  <si>
-    <t>ananyaiyengar@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hi! My name is Ananya and I initiated in my sophomore fall with the Alpha Sigma class. In my free time, I love to sing, try new sweet treats, and go to the beach. At recruitment, ask me about my favorite shows to binge-watch and why monkeys are my favorite animals. So excited to meet you all!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shreya </t>
-  </si>
-  <si>
-    <t>Jagannathan</t>
-  </si>
-  <si>
-    <t>shreya_jagannathan</t>
-  </si>
-  <si>
-    <t>San Ramon, CA</t>
-  </si>
-  <si>
-    <t>Business Information Management, Political Science</t>
-  </si>
-  <si>
-    <t>Law, Entrepreneurship, Finance</t>
-  </si>
-  <si>
-    <t>External Relations Assistant @ UCI Libraries</t>
-  </si>
-  <si>
-    <t>ASUCI</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/shreyajagan/</t>
-  </si>
-  <si>
-    <t>shreyajagannathan@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hey, my name is Shreya! I initiated in the fall quarter of my first year with the Alpha Sigma class. In my free time, I love to read, watch horror movies, and make very specific pinterest boards. Feel free to ask me about places I’ve traveled to and lived in!</t>
-  </si>
-  <si>
-    <t>Amelia</t>
-  </si>
-  <si>
-    <t>Jukita</t>
-  </si>
-  <si>
-    <t>amelia_jukita</t>
-  </si>
-  <si>
-    <t>Jakarta, Indonesia</t>
-  </si>
-  <si>
-    <t>Product Management</t>
-  </si>
-  <si>
-    <t>Product Management Intern @ Stride</t>
-  </si>
-  <si>
-    <t>180 Degrees Consulting, Product Association, MAISS</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/amelia-jukita/</t>
-  </si>
-  <si>
-    <t>ameliajukita@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hii! My name is Amelia, and I initiated in the fall quarter of my sophomore year with the Alpha Sigma Class. I enjoy thrifting, playing the piano, and exploring new food combinations. Feel free to ask me about my love for harbor seals!</t>
-  </si>
-  <si>
-    <t>Riya</t>
-  </si>
-  <si>
-    <t>Kapadekar</t>
-  </si>
-  <si>
-    <t>riya_kapadekar</t>
-  </si>
-  <si>
-    <t>Informatics</t>
-  </si>
-  <si>
-    <t>Psychology</t>
-  </si>
-  <si>
-    <t>Project Management, Product Management</t>
-  </si>
-  <si>
-    <t>Specialty Masters Program Student Assistant @ Paul Merage School of Business</t>
-  </si>
-  <si>
-    <t>MAISS, Product Association</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/riya-kapadekar/</t>
-  </si>
-  <si>
-    <t>riyakapadekar@ucidsp.com</t>
-  </si>
-  <si>
-    <t>Hi! My name is Riya and I'm part of the Alpha Sigma class. In my free time, I love going to the beach, making Pinterest boards, and trying new cafes! Ask me about my love for Tru Fru, Lana del Rey, and Grey's Anatomy.</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kent</t>
-  </si>
-  <si>
-    <t>james_kent</t>
-  </si>
-  <si>
-    <t>Santa Clarita, CA</t>
-  </si>
-  <si>
-    <t>Economics</t>
   </si>
   <si>
     <t>Asset &amp; Wealth Management</t>
@@ -2907,10 +2907,10 @@
         <v>195</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>197</v>
@@ -3343,7 +3343,7 @@
         <v>195</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
@@ -3915,7 +3915,7 @@
         <v>390</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="18" t="s">
@@ -4529,7 +4529,7 @@
         <v>195</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="I47" s="18" t="s">
         <v>319</v>

</xml_diff>